<commit_message>
Edited Title Names for Graphs
</commit_message>
<xml_diff>
--- a/Documents/BurnDown.xlsx
+++ b/Documents/BurnDown.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17927"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lewis/GitHub/IFB299/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Xero\Documents\GitHub\IFB299\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,16 +14,16 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -86,7 +86,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -227,15 +227,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="14">
@@ -254,8 +254,36 @@
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -268,7 +296,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -302,7 +330,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Media Vault Burndown</a:t>
+              <a:t>Sprint Burndown</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -312,7 +340,7 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.434751999434414"/>
-          <c:y val="0.0179568978084167"/>
+          <c:y val="1.7956897808416701E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -406,9 +434,8 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -433,67 +460,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11.0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12.0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>13.0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>14.0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>15.0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>17.0</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>18.0</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>19.0</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -505,31 +532,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>97.0</c:v>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>92.15000000000001</c:v>
+                  <c:v>92.15</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>87.30000000000001</c:v>
+                  <c:v>87.300000000000011</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>82.45</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>77.60000000000001</c:v>
+                  <c:v>77.600000000000009</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>72.75</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>67.9</c:v>
+                  <c:v>67.900000000000006</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>63.05</c:v>
+                  <c:v>63.050000000000004</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>58.2</c:v>
+                  <c:v>58.199999999999996</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>53.35</c:v>
@@ -541,10 +568,10 @@
                   <c:v>43.65</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>38.8</c:v>
+                  <c:v>38.799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>33.95</c:v>
+                  <c:v>33.949999999999996</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>29.1</c:v>
@@ -553,22 +580,22 @@
                   <c:v>24.25</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>19.4</c:v>
+                  <c:v>19.399999999999999</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>14.55</c:v>
+                  <c:v>14.549999999999999</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>9.700000000000001</c:v>
+                  <c:v>9.7000000000000011</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4.85</c:v>
+                  <c:v>4.8499999999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-96C9-40FD-B4D0-B5C928463CD3}"/>
             </c:ext>
@@ -632,7 +659,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -657,67 +683,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11.0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12.0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>13.0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>14.0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>15.0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>17.0</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>18.0</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>19.0</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -729,72 +755,77 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>97.0</c:v>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>89.0</c:v>
+                  <c:v>89</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>86.0</c:v>
+                  <c:v>86</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>82.0</c:v>
+                  <c:v>82</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>76.0</c:v>
+                  <c:v>76</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>76.0</c:v>
+                  <c:v>76</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>72.0</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>68.0</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>62.0</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>56.0</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>49.0</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43.0</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>35.0</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>30.0</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>28.0</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>24.0</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>18.0</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>14.0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-EC0F-49DD-B517-3E6C88D80309}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:dLblPos val="ctr"/>
@@ -857,7 +888,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -964,7 +994,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1087,7 +1116,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1121,12 +1150,19 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Sprint Burndown</a:t>
+              <a:t>Release</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Burndown</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1207,13 +1243,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1225,18 +1261,23 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>28.0</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14.0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-42BC-4F89-8350-B29AE1F55494}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1275,15 +1316,20 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>28.0</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14.0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-42BC-4F89-8350-B29AE1F55494}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1336,7 +1382,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1462,7 +1507,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1492,6 +1536,7 @@
             </a:p>
           </c:txPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2709,7 +2754,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2739,7 +2790,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -3023,23 +3080,23 @@
   <dimension ref="B1:W23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="99" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="J43" sqref="J43"/>
+      <selection activeCell="Y24" sqref="Y24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="28.33203125" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" customWidth="1"/>
-    <col min="9" max="9" width="10.83203125" customWidth="1"/>
-    <col min="10" max="10" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="28.36328125" customWidth="1"/>
+    <col min="3" max="3" width="13.36328125" customWidth="1"/>
+    <col min="9" max="9" width="10.81640625" customWidth="1"/>
+    <col min="10" max="10" width="15.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -3126,7 +3183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
@@ -3194,7 +3251,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>2</v>
       </c>
@@ -3262,12 +3319,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B6" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
@@ -3281,7 +3338,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B8" s="2" t="s">
         <v>14</v>
       </c>
@@ -3295,7 +3352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B9" s="2" t="s">
         <v>15</v>
       </c>
@@ -3306,156 +3363,156 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="2:16" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:16" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
-      <c r="E17" s="5" t="s">
+      <c r="E17" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
       <c r="M17" s="4"/>
       <c r="N17" s="4"/>
       <c r="O17" s="4"/>
       <c r="P17" s="4"/>
     </row>
-    <row r="18" spans="2:16" ht="16" x14ac:dyDescent="0.2">
-      <c r="B18" s="6" t="s">
+    <row r="18" spans="2:16" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B18" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="7" t="s">
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="8"/>
-      <c r="M18" s="7" t="s">
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="N18" s="7"/>
-      <c r="O18" s="7"/>
-      <c r="P18" s="7"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="6"/>
+      <c r="P18" s="6"/>
     </row>
-    <row r="19" spans="2:16" ht="16" x14ac:dyDescent="0.2">
-      <c r="B19" s="6" t="s">
+    <row r="19" spans="2:16" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B19" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="9">
+      <c r="C19" s="8">
         <v>4</v>
       </c>
-      <c r="D19" s="9">
+      <c r="D19" s="8">
         <v>7</v>
       </c>
-      <c r="E19" s="9">
+      <c r="E19" s="8">
         <v>6</v>
       </c>
-      <c r="F19" s="9">
+      <c r="F19" s="8">
         <v>5</v>
       </c>
-      <c r="G19" s="8"/>
-      <c r="H19" s="9">
+      <c r="G19" s="7"/>
+      <c r="H19" s="8">
         <v>20</v>
       </c>
-      <c r="I19" s="9">
+      <c r="I19" s="8">
         <v>6</v>
       </c>
-      <c r="J19" s="10" t="s">
+      <c r="J19" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="K19" s="9">
+      <c r="K19" s="8">
         <v>18</v>
       </c>
-      <c r="L19" s="8"/>
-      <c r="M19" s="9">
+      <c r="L19" s="7"/>
+      <c r="M19" s="8">
         <v>1</v>
       </c>
-      <c r="N19" s="9">
+      <c r="N19" s="8">
         <v>3</v>
       </c>
-      <c r="O19" s="9">
+      <c r="O19" s="8">
         <v>13</v>
       </c>
-      <c r="P19" s="9">
+      <c r="P19" s="8">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="2:16" ht="16" x14ac:dyDescent="0.2">
-      <c r="B20" s="6" t="s">
+    <row r="20" spans="2:16" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B20" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="8">
+      <c r="C20" s="7">
         <v>2</v>
       </c>
-      <c r="D20" s="8">
+      <c r="D20" s="7">
         <v>1</v>
       </c>
-      <c r="E20" s="8">
+      <c r="E20" s="7">
         <v>1</v>
       </c>
-      <c r="F20" s="8">
+      <c r="F20" s="7">
         <v>1</v>
       </c>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8">
+      <c r="G20" s="7"/>
+      <c r="H20" s="7">
         <v>1</v>
       </c>
-      <c r="I20" s="8">
+      <c r="I20" s="7">
         <v>1</v>
       </c>
-      <c r="J20" s="8">
+      <c r="J20" s="7">
         <v>2</v>
       </c>
-      <c r="K20" s="8">
+      <c r="K20" s="7">
         <v>1</v>
       </c>
-      <c r="L20" s="8"/>
-      <c r="M20" s="8">
+      <c r="L20" s="7"/>
+      <c r="M20" s="7">
         <v>1</v>
       </c>
-      <c r="N20" s="8">
+      <c r="N20" s="7">
         <v>1</v>
       </c>
-      <c r="O20" s="8">
+      <c r="O20" s="7">
         <v>1</v>
       </c>
-      <c r="P20" s="8">
+      <c r="P20" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="2:16" ht="16" x14ac:dyDescent="0.2">
-      <c r="B21" s="6" t="s">
+    <row r="21" spans="2:16" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B21" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="8"/>
-      <c r="K21" s="8"/>
-      <c r="L21" s="8"/>
-      <c r="M21" s="8"/>
-      <c r="N21" s="8"/>
-      <c r="O21" s="8"/>
-      <c r="P21" s="8"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="7"/>
+      <c r="M21" s="7"/>
+      <c r="N21" s="7"/>
+      <c r="O21" s="7"/>
+      <c r="P21" s="7"/>
     </row>
-    <row r="23" spans="2:16" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:16" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C23" s="3" t="s">
         <v>9</v>
       </c>

</xml_diff>